<commit_message>
Added variable type columns
Show good, useless, and bad controls column
</commit_message>
<xml_diff>
--- a/HW3/Codebook.xlsx
+++ b/HW3/Codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\.spyder-py3\SS340_Abdelwahed\HW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7073DD1-32AF-4B84-900B-ED0BDA05DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F1A220-FE92-43B7-B617-489025606C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1655C110-EC22-4A30-96D6-58EB43745179}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>original</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>whitefather</t>
+  </si>
+  <si>
+    <t>predicted type</t>
+  </si>
+  <si>
+    <t>useless</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>bad</t>
   </si>
 </sst>
 </file>
@@ -538,19 +550,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F257E36B-ABBF-4D7C-97E1-570DBDB42A50}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +577,11 @@
       <c r="D1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -574,8 +591,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -588,8 +608,11 @@
       <c r="D3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -602,8 +625,11 @@
       <c r="D4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -613,8 +639,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -627,8 +656,11 @@
       <c r="D6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -638,8 +670,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -652,8 +687,11 @@
       <c r="D8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -664,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -674,8 +712,11 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -686,7 +727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -699,8 +740,11 @@
       <c r="D12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -710,8 +754,11 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -724,8 +771,11 @@
       <c r="D14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -738,8 +788,11 @@
       <c r="D15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -748,6 +801,9 @@
       </c>
       <c r="C16" t="s">
         <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>